<commit_message>
Edits for making final version of the paper figures committed.
</commit_message>
<xml_diff>
--- a/relevant_data/mitchell_data_all/orig_download/aff_data_2_w_amp/afferent_data_updated.xlsx
+++ b/relevant_data/mitchell_data_all/orig_download/aff_data_2_w_amp/afferent_data_updated.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10114"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mitdia00\Desktop\afferent_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cynthiasteinhardt/Dropbox/coding_reservoirs/code_directories/pulsatileDir/relevant_data/mitchell_data_all/orig_download/aff_data_2_w_amp/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47AEA472-586F-D04A-8614-A5020C094ACC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="14100"/>
+    <workbookView xWindow="-1880" yWindow="-18420" windowWidth="34540" windowHeight="17680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -120,7 +121,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -187,7 +188,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -223,11 +224,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -248,13 +260,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -263,10 +268,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -301,7 +309,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Image 1" descr="https://attachments.office.net/owa/diana.mitchell%40mail.mcgill.ca/service.svc/s/GetAttachmentThumbnail?id=AAMkADc5MmE1MmYyLTdhNTUtNDhiNC05MzYzLWE1YjA5NWQyYzI0MwBGAAAAAADugN8DkS4MTL3ZuC%2B%2F5KU6BwB%2B5KHRNU0TSrhtGx73W2sFAAAABALUAAD7yC0FYtZ%2FRo4NqLo9fdP9AAK8QyQLAAABEgAQAH4l1rXtW5xLiDsYpv5p0zE%3D&amp;thumbnailType=2&amp;owa=outlook.office.com&amp;scriptVer=20201019001.14&amp;X-OWA-CANARY=_US3hWEPgku74g-HWPxCcYC2CMhLfNgYKyKNvzMLIDYYdbG3kJA1sCPLdfT3-6gcJOxhSMs5S1k.&amp;token=eyJhbGciOiJSUzI1NiIsImtpZCI6IjU2MzU4ODUyMzRCOTI1MkRERTAwNTc2NkQ5RDlGMjc2NTY1RjYzRTIiLCJ0eXAiOiJKV1QiLCJ4NXQiOiJWaldJVWpTNUpTM2VBRmRtMmRueWRsWmZZLUkifQ.eyJvcmlnaW4iOiJodHRwczovL291dGxvb2sub2ZmaWNlLmNvbSIsInVjIjoiZWVmMTQ3NDllMzJjNGMxNWFlNjI0NzAzM2E0Yjg4ZTgiLCJzaWduaW5fc3RhdGUiOiJbXCJrbXNpXCJdIiwidmVyIjoiRXhjaGFuZ2UuQ2FsbGJhY2suVjEiLCJhcHBjdHhzZW5kZXIiOiJPd2FEb3dubG9hZEBjZDMxOTY3MS01MmU3LTRhNjgtYWZhOS1mY2Y4Zjg5ZjA5ZWEiLCJpc3NyaW5nIjoiV1ciLCJhcHBjdHgiOiJ7XCJtc2V4Y2hwcm90XCI6XCJvd2FcIixcInByaW1hcnlzaWRcIjpcIlMtMS01LTIxLTM5NzE5NTY3OC0xOTY5Njg2MjMxLTIyMjY0NjU5MC04MzkyOTc1XCIsXCJwdWlkXCI6XCIxMTUzODM2Mjk2MzE3ODYwMTg1XCIsXCJvaWRcIjpcIjFjYjEwZjM3LTc1MjgtNDQ2OS04YzU2LTcyM2YzNTEwNGVlYlwiLFwic2NvcGVcIjpcIk93YURvd25sb2FkXCJ9IiwibmJmIjoxNjA0MDA0MzAyLCJleHAiOjE2MDQwMDQ5MDIsImlzcyI6IjAwMDAwMDAyLTAwMDAtMGZmMS1jZTAwLTAwMDAwMDAwMDAwMEBjZDMxOTY3MS01MmU3LTRhNjgtYWZhOS1mY2Y4Zjg5ZjA5ZWEiLCJhdWQiOiIwMDAwMDAwMi0wMDAwLTBmZjEtY2UwMC0wMDAwMDAwMDAwMDAvYXR0YWNobWVudHMub2ZmaWNlLm5ldEBjZDMxOTY3MS01MmU3LTRhNjgtYWZhOS1mY2Y4Zjg5ZjA5ZWEiLCJoYXBwIjoib3dhIn0.gZ9dxAmPm3zZ0MELyOjVDXXmxIV7idcNLv-8Nycxs68J7cEtpokrH6P6CC74G_qaJlcxd2M7fxupSnalOGils37JnsMaaWoTh1Zrnulna2aCyiTgMuq16WZllTHGUajm_gQSygm4xslvqoI_YoJw8-2jqcOeTYaosC7wXXoCwUmsJv-emhWwn4APhcpmVvhPlQUExsktBZa_5-GiAPgNoE1zNqZfce8VSN1GTY-INW6wBUbXMPH1aDdgkKWoH6GnNagvEyteS0HCZNiOedm6ZGNpFjPg0Rf4l5Vnu8PIgcSC9oeKTGxXBeqWJQU-SdZeOhqEdtr755QqWBlcuZ9qdw&amp;animation=true"/>
+        <xdr:cNvPr id="2" name="Image 1" descr="https://attachments.office.net/owa/diana.mitchell%40mail.mcgill.ca/service.svc/s/GetAttachmentThumbnail?id=AAMkADc5MmE1MmYyLTdhNTUtNDhiNC05MzYzLWE1YjA5NWQyYzI0MwBGAAAAAADugN8DkS4MTL3ZuC%2B%2F5KU6BwB%2B5KHRNU0TSrhtGx73W2sFAAAABALUAAD7yC0FYtZ%2FRo4NqLo9fdP9AAK8QyQLAAABEgAQAH4l1rXtW5xLiDsYpv5p0zE%3D&amp;thumbnailType=2&amp;owa=outlook.office.com&amp;scriptVer=20201019001.14&amp;X-OWA-CANARY=_US3hWEPgku74g-HWPxCcYC2CMhLfNgYKyKNvzMLIDYYdbG3kJA1sCPLdfT3-6gcJOxhSMs5S1k.&amp;token=eyJhbGciOiJSUzI1NiIsImtpZCI6IjU2MzU4ODUyMzRCOTI1MkRERTAwNTc2NkQ5RDlGMjc2NTY1RjYzRTIiLCJ0eXAiOiJKV1QiLCJ4NXQiOiJWaldJVWpTNUpTM2VBRmRtMmRueWRsWmZZLUkifQ.eyJvcmlnaW4iOiJodHRwczovL291dGxvb2sub2ZmaWNlLmNvbSIsInVjIjoiZWVmMTQ3NDllMzJjNGMxNWFlNjI0NzAzM2E0Yjg4ZTgiLCJzaWduaW5fc3RhdGUiOiJbXCJrbXNpXCJdIiwidmVyIjoiRXhjaGFuZ2UuQ2FsbGJhY2suVjEiLCJhcHBjdHhzZW5kZXIiOiJPd2FEb3dubG9hZEBjZDMxOTY3MS01MmU3LTRhNjgtYWZhOS1mY2Y4Zjg5ZjA5ZWEiLCJpc3NyaW5nIjoiV1ciLCJhcHBjdHgiOiJ7XCJtc2V4Y2hwcm90XCI6XCJvd2FcIixcInByaW1hcnlzaWRcIjpcIlMtMS01LTIxLTM5NzE5NTY3OC0xOTY5Njg2MjMxLTIyMjY0NjU5MC04MzkyOTc1XCIsXCJwdWlkXCI6XCIxMTUzODM2Mjk2MzE3ODYwMTg1XCIsXCJvaWRcIjpcIjFjYjEwZjM3LTc1MjgtNDQ2OS04YzU2LTcyM2YzNTEwNGVlYlwiLFwic2NvcGVcIjpcIk93YURvd25sb2FkXCJ9IiwibmJmIjoxNjA0MDA0MzAyLCJleHAiOjE2MDQwMDQ5MDIsImlzcyI6IjAwMDAwMDAyLTAwMDAtMGZmMS1jZTAwLTAwMDAwMDAwMDAwMEBjZDMxOTY3MS01MmU3LTRhNjgtYWZhOS1mY2Y4Zjg5ZjA5ZWEiLCJhdWQiOiIwMDAwMDAwMi0wMDAwLTBmZjEtY2UwMC0wMDAwMDAwMDAwMDAvYXR0YWNobWVudHMub2ZmaWNlLm5ldEBjZDMxOTY3MS01MmU3LTRhNjgtYWZhOS1mY2Y4Zjg5ZjA5ZWEiLCJoYXBwIjoib3dhIn0.gZ9dxAmPm3zZ0MELyOjVDXXmxIV7idcNLv-8Nycxs68J7cEtpokrH6P6CC74G_qaJlcxd2M7fxupSnalOGils37JnsMaaWoTh1Zrnulna2aCyiTgMuq16WZllTHGUajm_gQSygm4xslvqoI_YoJw8-2jqcOeTYaosC7wXXoCwUmsJv-emhWwn4APhcpmVvhPlQUExsktBZa_5-GiAPgNoE1zNqZfce8VSN1GTY-INW6wBUbXMPH1aDdgkKWoH6GnNagvEyteS0HCZNiOedm6ZGNpFjPg0Rf4l5Vnu8PIgcSC9oeKTGxXBeqWJQU-SdZeOhqEdtr755QqWBlcuZ9qdw&amp;animation=true">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -356,7 +370,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Image 2" descr="https://attachments.office.net/owa/diana.mitchell%40mail.mcgill.ca/service.svc/s/GetAttachmentThumbnail?id=AAMkADc5MmE1MmYyLTdhNTUtNDhiNC05MzYzLWE1YjA5NWQyYzI0MwBGAAAAAADugN8DkS4MTL3ZuC%2B%2F5KU6BwB%2B5KHRNU0TSrhtGx73W2sFAAAABALUAAD7yC0FYtZ%2FRo4NqLo9fdP9AAK8QyQLAAABEgAQACtdRsClMmBGrwo35pWrjnA%3D&amp;thumbnailType=2&amp;owa=outlook.office.com&amp;scriptVer=20201019001.14&amp;X-OWA-CANARY=_US3hWEPgku74g-HWPxCcYC2CMhLfNgYKyKNvzMLIDYYdbG3kJA1sCPLdfT3-6gcJOxhSMs5S1k.&amp;token=eyJhbGciOiJSUzI1NiIsImtpZCI6IjU2MzU4ODUyMzRCOTI1MkRERTAwNTc2NkQ5RDlGMjc2NTY1RjYzRTIiLCJ0eXAiOiJKV1QiLCJ4NXQiOiJWaldJVWpTNUpTM2VBRmRtMmRueWRsWmZZLUkifQ.eyJvcmlnaW4iOiJodHRwczovL291dGxvb2sub2ZmaWNlLmNvbSIsInVjIjoiZWVmMTQ3NDllMzJjNGMxNWFlNjI0NzAzM2E0Yjg4ZTgiLCJzaWduaW5fc3RhdGUiOiJbXCJrbXNpXCJdIiwidmVyIjoiRXhjaGFuZ2UuQ2FsbGJhY2suVjEiLCJhcHBjdHhzZW5kZXIiOiJPd2FEb3dubG9hZEBjZDMxOTY3MS01MmU3LTRhNjgtYWZhOS1mY2Y4Zjg5ZjA5ZWEiLCJpc3NyaW5nIjoiV1ciLCJhcHBjdHgiOiJ7XCJtc2V4Y2hwcm90XCI6XCJvd2FcIixcInByaW1hcnlzaWRcIjpcIlMtMS01LTIxLTM5NzE5NTY3OC0xOTY5Njg2MjMxLTIyMjY0NjU5MC04MzkyOTc1XCIsXCJwdWlkXCI6XCIxMTUzODM2Mjk2MzE3ODYwMTg1XCIsXCJvaWRcIjpcIjFjYjEwZjM3LTc1MjgtNDQ2OS04YzU2LTcyM2YzNTEwNGVlYlwiLFwic2NvcGVcIjpcIk93YURvd25sb2FkXCJ9IiwibmJmIjoxNjA0MDA0MzAyLCJleHAiOjE2MDQwMDQ5MDIsImlzcyI6IjAwMDAwMDAyLTAwMDAtMGZmMS1jZTAwLTAwMDAwMDAwMDAwMEBjZDMxOTY3MS01MmU3LTRhNjgtYWZhOS1mY2Y4Zjg5ZjA5ZWEiLCJhdWQiOiIwMDAwMDAwMi0wMDAwLTBmZjEtY2UwMC0wMDAwMDAwMDAwMDAvYXR0YWNobWVudHMub2ZmaWNlLm5ldEBjZDMxOTY3MS01MmU3LTRhNjgtYWZhOS1mY2Y4Zjg5ZjA5ZWEiLCJoYXBwIjoib3dhIn0.gZ9dxAmPm3zZ0MELyOjVDXXmxIV7idcNLv-8Nycxs68J7cEtpokrH6P6CC74G_qaJlcxd2M7fxupSnalOGils37JnsMaaWoTh1Zrnulna2aCyiTgMuq16WZllTHGUajm_gQSygm4xslvqoI_YoJw8-2jqcOeTYaosC7wXXoCwUmsJv-emhWwn4APhcpmVvhPlQUExsktBZa_5-GiAPgNoE1zNqZfce8VSN1GTY-INW6wBUbXMPH1aDdgkKWoH6GnNagvEyteS0HCZNiOedm6ZGNpFjPg0Rf4l5Vnu8PIgcSC9oeKTGxXBeqWJQU-SdZeOhqEdtr755QqWBlcuZ9qdw&amp;animation=true"/>
+        <xdr:cNvPr id="3" name="Image 2" descr="https://attachments.office.net/owa/diana.mitchell%40mail.mcgill.ca/service.svc/s/GetAttachmentThumbnail?id=AAMkADc5MmE1MmYyLTdhNTUtNDhiNC05MzYzLWE1YjA5NWQyYzI0MwBGAAAAAADugN8DkS4MTL3ZuC%2B%2F5KU6BwB%2B5KHRNU0TSrhtGx73W2sFAAAABALUAAD7yC0FYtZ%2FRo4NqLo9fdP9AAK8QyQLAAABEgAQACtdRsClMmBGrwo35pWrjnA%3D&amp;thumbnailType=2&amp;owa=outlook.office.com&amp;scriptVer=20201019001.14&amp;X-OWA-CANARY=_US3hWEPgku74g-HWPxCcYC2CMhLfNgYKyKNvzMLIDYYdbG3kJA1sCPLdfT3-6gcJOxhSMs5S1k.&amp;token=eyJhbGciOiJSUzI1NiIsImtpZCI6IjU2MzU4ODUyMzRCOTI1MkRERTAwNTc2NkQ5RDlGMjc2NTY1RjYzRTIiLCJ0eXAiOiJKV1QiLCJ4NXQiOiJWaldJVWpTNUpTM2VBRmRtMmRueWRsWmZZLUkifQ.eyJvcmlnaW4iOiJodHRwczovL291dGxvb2sub2ZmaWNlLmNvbSIsInVjIjoiZWVmMTQ3NDllMzJjNGMxNWFlNjI0NzAzM2E0Yjg4ZTgiLCJzaWduaW5fc3RhdGUiOiJbXCJrbXNpXCJdIiwidmVyIjoiRXhjaGFuZ2UuQ2FsbGJhY2suVjEiLCJhcHBjdHhzZW5kZXIiOiJPd2FEb3dubG9hZEBjZDMxOTY3MS01MmU3LTRhNjgtYWZhOS1mY2Y4Zjg5ZjA5ZWEiLCJpc3NyaW5nIjoiV1ciLCJhcHBjdHgiOiJ7XCJtc2V4Y2hwcm90XCI6XCJvd2FcIixcInByaW1hcnlzaWRcIjpcIlMtMS01LTIxLTM5NzE5NTY3OC0xOTY5Njg2MjMxLTIyMjY0NjU5MC04MzkyOTc1XCIsXCJwdWlkXCI6XCIxMTUzODM2Mjk2MzE3ODYwMTg1XCIsXCJvaWRcIjpcIjFjYjEwZjM3LTc1MjgtNDQ2OS04YzU2LTcyM2YzNTEwNGVlYlwiLFwic2NvcGVcIjpcIk93YURvd25sb2FkXCJ9IiwibmJmIjoxNjA0MDA0MzAyLCJleHAiOjE2MDQwMDQ5MDIsImlzcyI6IjAwMDAwMDAyLTAwMDAtMGZmMS1jZTAwLTAwMDAwMDAwMDAwMEBjZDMxOTY3MS01MmU3LTRhNjgtYWZhOS1mY2Y4Zjg5ZjA5ZWEiLCJhdWQiOiIwMDAwMDAwMi0wMDAwLTBmZjEtY2UwMC0wMDAwMDAwMDAwMDAvYXR0YWNobWVudHMub2ZmaWNlLm5ldEBjZDMxOTY3MS01MmU3LTRhNjgtYWZhOS1mY2Y4Zjg5ZjA5ZWEiLCJoYXBwIjoib3dhIn0.gZ9dxAmPm3zZ0MELyOjVDXXmxIV7idcNLv-8Nycxs68J7cEtpokrH6P6CC74G_qaJlcxd2M7fxupSnalOGils37JnsMaaWoTh1Zrnulna2aCyiTgMuq16WZllTHGUajm_gQSygm4xslvqoI_YoJw8-2jqcOeTYaosC7wXXoCwUmsJv-emhWwn4APhcpmVvhPlQUExsktBZa_5-GiAPgNoE1zNqZfce8VSN1GTY-INW6wBUbXMPH1aDdgkKWoH6GnNagvEyteS0HCZNiOedm6ZGNpFjPg0Rf4l5Vnu8PIgcSC9oeKTGxXBeqWJQU-SdZeOhqEdtr755QqWBlcuZ9qdw&amp;animation=true">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -411,7 +431,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Image 3" descr="https://attachments.office.net/owa/diana.mitchell%40mail.mcgill.ca/service.svc/s/GetAttachmentThumbnail?id=AAMkADc5MmE1MmYyLTdhNTUtNDhiNC05MzYzLWE1YjA5NWQyYzI0MwBGAAAAAADugN8DkS4MTL3ZuC%2B%2F5KU6BwB%2B5KHRNU0TSrhtGx73W2sFAAAABALUAAD7yC0FYtZ%2FRo4NqLo9fdP9AAK8QyQLAAABEgAQAPVOZ87XaaZCv7tre8ECrGA%3D&amp;thumbnailType=2&amp;owa=outlook.office.com&amp;scriptVer=20201019001.14&amp;X-OWA-CANARY=h4550aTPSUGIWZ1UvN4kH7DGmxdMfNgYStjoh27XBHMBRQ8ae1FCs64E9kJbeIMqXjUDbprf-Dc.&amp;token=eyJhbGciOiJSUzI1NiIsImtpZCI6IjU2MzU4ODUyMzRCOTI1MkRERTAwNTc2NkQ5RDlGMjc2NTY1RjYzRTIiLCJ0eXAiOiJKV1QiLCJ4NXQiOiJWaldJVWpTNUpTM2VBRmRtMmRueWRsWmZZLUkifQ.eyJvcmlnaW4iOiJodHRwczovL291dGxvb2sub2ZmaWNlLmNvbSIsInVjIjoiZWVmMTQ3NDllMzJjNGMxNWFlNjI0NzAzM2E0Yjg4ZTgiLCJzaWduaW5fc3RhdGUiOiJbXCJrbXNpXCJdIiwidmVyIjoiRXhjaGFuZ2UuQ2FsbGJhY2suVjEiLCJhcHBjdHhzZW5kZXIiOiJPd2FEb3dubG9hZEBjZDMxOTY3MS01MmU3LTRhNjgtYWZhOS1mY2Y4Zjg5ZjA5ZWEiLCJpc3NyaW5nIjoiV1ciLCJhcHBjdHgiOiJ7XCJtc2V4Y2hwcm90XCI6XCJvd2FcIixcInByaW1hcnlzaWRcIjpcIlMtMS01LTIxLTM5NzE5NTY3OC0xOTY5Njg2MjMxLTIyMjY0NjU5MC04MzkyOTc1XCIsXCJwdWlkXCI6XCIxMTUzODM2Mjk2MzE3ODYwMTg1XCIsXCJvaWRcIjpcIjFjYjEwZjM3LTc1MjgtNDQ2OS04YzU2LTcyM2YzNTEwNGVlYlwiLFwic2NvcGVcIjpcIk93YURvd25sb2FkXCJ9IiwibmJmIjoxNjA0MDA0MzAyLCJleHAiOjE2MDQwMDQ5MDIsImlzcyI6IjAwMDAwMDAyLTAwMDAtMGZmMS1jZTAwLTAwMDAwMDAwMDAwMEBjZDMxOTY3MS01MmU3LTRhNjgtYWZhOS1mY2Y4Zjg5ZjA5ZWEiLCJhdWQiOiIwMDAwMDAwMi0wMDAwLTBmZjEtY2UwMC0wMDAwMDAwMDAwMDAvYXR0YWNobWVudHMub2ZmaWNlLm5ldEBjZDMxOTY3MS01MmU3LTRhNjgtYWZhOS1mY2Y4Zjg5ZjA5ZWEiLCJoYXBwIjoib3dhIn0.gZ9dxAmPm3zZ0MELyOjVDXXmxIV7idcNLv-8Nycxs68J7cEtpokrH6P6CC74G_qaJlcxd2M7fxupSnalOGils37JnsMaaWoTh1Zrnulna2aCyiTgMuq16WZllTHGUajm_gQSygm4xslvqoI_YoJw8-2jqcOeTYaosC7wXXoCwUmsJv-emhWwn4APhcpmVvhPlQUExsktBZa_5-GiAPgNoE1zNqZfce8VSN1GTY-INW6wBUbXMPH1aDdgkKWoH6GnNagvEyteS0HCZNiOedm6ZGNpFjPg0Rf4l5Vnu8PIgcSC9oeKTGxXBeqWJQU-SdZeOhqEdtr755QqWBlcuZ9qdw&amp;animation=true"/>
+        <xdr:cNvPr id="4" name="Image 3" descr="https://attachments.office.net/owa/diana.mitchell%40mail.mcgill.ca/service.svc/s/GetAttachmentThumbnail?id=AAMkADc5MmE1MmYyLTdhNTUtNDhiNC05MzYzLWE1YjA5NWQyYzI0MwBGAAAAAADugN8DkS4MTL3ZuC%2B%2F5KU6BwB%2B5KHRNU0TSrhtGx73W2sFAAAABALUAAD7yC0FYtZ%2FRo4NqLo9fdP9AAK8QyQLAAABEgAQAPVOZ87XaaZCv7tre8ECrGA%3D&amp;thumbnailType=2&amp;owa=outlook.office.com&amp;scriptVer=20201019001.14&amp;X-OWA-CANARY=h4550aTPSUGIWZ1UvN4kH7DGmxdMfNgYStjoh27XBHMBRQ8ae1FCs64E9kJbeIMqXjUDbprf-Dc.&amp;token=eyJhbGciOiJSUzI1NiIsImtpZCI6IjU2MzU4ODUyMzRCOTI1MkRERTAwNTc2NkQ5RDlGMjc2NTY1RjYzRTIiLCJ0eXAiOiJKV1QiLCJ4NXQiOiJWaldJVWpTNUpTM2VBRmRtMmRueWRsWmZZLUkifQ.eyJvcmlnaW4iOiJodHRwczovL291dGxvb2sub2ZmaWNlLmNvbSIsInVjIjoiZWVmMTQ3NDllMzJjNGMxNWFlNjI0NzAzM2E0Yjg4ZTgiLCJzaWduaW5fc3RhdGUiOiJbXCJrbXNpXCJdIiwidmVyIjoiRXhjaGFuZ2UuQ2FsbGJhY2suVjEiLCJhcHBjdHhzZW5kZXIiOiJPd2FEb3dubG9hZEBjZDMxOTY3MS01MmU3LTRhNjgtYWZhOS1mY2Y4Zjg5ZjA5ZWEiLCJpc3NyaW5nIjoiV1ciLCJhcHBjdHgiOiJ7XCJtc2V4Y2hwcm90XCI6XCJvd2FcIixcInByaW1hcnlzaWRcIjpcIlMtMS01LTIxLTM5NzE5NTY3OC0xOTY5Njg2MjMxLTIyMjY0NjU5MC04MzkyOTc1XCIsXCJwdWlkXCI6XCIxMTUzODM2Mjk2MzE3ODYwMTg1XCIsXCJvaWRcIjpcIjFjYjEwZjM3LTc1MjgtNDQ2OS04YzU2LTcyM2YzNTEwNGVlYlwiLFwic2NvcGVcIjpcIk93YURvd25sb2FkXCJ9IiwibmJmIjoxNjA0MDA0MzAyLCJleHAiOjE2MDQwMDQ5MDIsImlzcyI6IjAwMDAwMDAyLTAwMDAtMGZmMS1jZTAwLTAwMDAwMDAwMDAwMEBjZDMxOTY3MS01MmU3LTRhNjgtYWZhOS1mY2Y4Zjg5ZjA5ZWEiLCJhdWQiOiIwMDAwMDAwMi0wMDAwLTBmZjEtY2UwMC0wMDAwMDAwMDAwMDAvYXR0YWNobWVudHMub2ZmaWNlLm5ldEBjZDMxOTY3MS01MmU3LTRhNjgtYWZhOS1mY2Y4Zjg5ZjA5ZWEiLCJoYXBwIjoib3dhIn0.gZ9dxAmPm3zZ0MELyOjVDXXmxIV7idcNLv-8Nycxs68J7cEtpokrH6P6CC74G_qaJlcxd2M7fxupSnalOGils37JnsMaaWoTh1Zrnulna2aCyiTgMuq16WZllTHGUajm_gQSygm4xslvqoI_YoJw8-2jqcOeTYaosC7wXXoCwUmsJv-emhWwn4APhcpmVvhPlQUExsktBZa_5-GiAPgNoE1zNqZfce8VSN1GTY-INW6wBUbXMPH1aDdgkKWoH6GnNagvEyteS0HCZNiOedm6ZGNpFjPg0Rf4l5Vnu8PIgcSC9oeKTGxXBeqWJQU-SdZeOhqEdtr755QqWBlcuZ9qdw&amp;animation=true">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -466,7 +492,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="Image 4" descr="https://attachments.office.net/owa/diana.mitchell%40mail.mcgill.ca/service.svc/s/GetAttachmentThumbnail?id=AAMkADc5MmE1MmYyLTdhNTUtNDhiNC05MzYzLWE1YjA5NWQyYzI0MwBGAAAAAADugN8DkS4MTL3ZuC%2B%2F5KU6BwB%2B5KHRNU0TSrhtGx73W2sFAAAABALUAAD7yC0FYtZ%2FRo4NqLo9fdP9AAK8QyQLAAABEgAQADCNtIDycrRAumEeiSaE5iM%3D&amp;thumbnailType=2&amp;owa=outlook.office.com&amp;scriptVer=20201019001.14&amp;X-OWA-CANARY=_nP35uPsQkqVCZYQJGBugPD3xy9MfNgY1KM3Rz3wAJPU4RjIEzcUfkGAJNwZSEODB-LjjAeQaqI.&amp;token=eyJhbGciOiJSUzI1NiIsImtpZCI6IjU2MzU4ODUyMzRCOTI1MkRERTAwNTc2NkQ5RDlGMjc2NTY1RjYzRTIiLCJ0eXAiOiJKV1QiLCJ4NXQiOiJWaldJVWpTNUpTM2VBRmRtMmRueWRsWmZZLUkifQ.eyJvcmlnaW4iOiJodHRwczovL291dGxvb2sub2ZmaWNlLmNvbSIsInVjIjoiZWVmMTQ3NDllMzJjNGMxNWFlNjI0NzAzM2E0Yjg4ZTgiLCJzaWduaW5fc3RhdGUiOiJbXCJrbXNpXCJdIiwidmVyIjoiRXhjaGFuZ2UuQ2FsbGJhY2suVjEiLCJhcHBjdHhzZW5kZXIiOiJPd2FEb3dubG9hZEBjZDMxOTY3MS01MmU3LTRhNjgtYWZhOS1mY2Y4Zjg5ZjA5ZWEiLCJpc3NyaW5nIjoiV1ciLCJhcHBjdHgiOiJ7XCJtc2V4Y2hwcm90XCI6XCJvd2FcIixcInByaW1hcnlzaWRcIjpcIlMtMS01LTIxLTM5NzE5NTY3OC0xOTY5Njg2MjMxLTIyMjY0NjU5MC04MzkyOTc1XCIsXCJwdWlkXCI6XCIxMTUzODM2Mjk2MzE3ODYwMTg1XCIsXCJvaWRcIjpcIjFjYjEwZjM3LTc1MjgtNDQ2OS04YzU2LTcyM2YzNTEwNGVlYlwiLFwic2NvcGVcIjpcIk93YURvd25sb2FkXCJ9IiwibmJmIjoxNjA0MDA0MzAyLCJleHAiOjE2MDQwMDQ5MDIsImlzcyI6IjAwMDAwMDAyLTAwMDAtMGZmMS1jZTAwLTAwMDAwMDAwMDAwMEBjZDMxOTY3MS01MmU3LTRhNjgtYWZhOS1mY2Y4Zjg5ZjA5ZWEiLCJhdWQiOiIwMDAwMDAwMi0wMDAwLTBmZjEtY2UwMC0wMDAwMDAwMDAwMDAvYXR0YWNobWVudHMub2ZmaWNlLm5ldEBjZDMxOTY3MS01MmU3LTRhNjgtYWZhOS1mY2Y4Zjg5ZjA5ZWEiLCJoYXBwIjoib3dhIn0.gZ9dxAmPm3zZ0MELyOjVDXXmxIV7idcNLv-8Nycxs68J7cEtpokrH6P6CC74G_qaJlcxd2M7fxupSnalOGils37JnsMaaWoTh1Zrnulna2aCyiTgMuq16WZllTHGUajm_gQSygm4xslvqoI_YoJw8-2jqcOeTYaosC7wXXoCwUmsJv-emhWwn4APhcpmVvhPlQUExsktBZa_5-GiAPgNoE1zNqZfce8VSN1GTY-INW6wBUbXMPH1aDdgkKWoH6GnNagvEyteS0HCZNiOedm6ZGNpFjPg0Rf4l5Vnu8PIgcSC9oeKTGxXBeqWJQU-SdZeOhqEdtr755QqWBlcuZ9qdw&amp;animation=true"/>
+        <xdr:cNvPr id="5" name="Image 4" descr="https://attachments.office.net/owa/diana.mitchell%40mail.mcgill.ca/service.svc/s/GetAttachmentThumbnail?id=AAMkADc5MmE1MmYyLTdhNTUtNDhiNC05MzYzLWE1YjA5NWQyYzI0MwBGAAAAAADugN8DkS4MTL3ZuC%2B%2F5KU6BwB%2B5KHRNU0TSrhtGx73W2sFAAAABALUAAD7yC0FYtZ%2FRo4NqLo9fdP9AAK8QyQLAAABEgAQADCNtIDycrRAumEeiSaE5iM%3D&amp;thumbnailType=2&amp;owa=outlook.office.com&amp;scriptVer=20201019001.14&amp;X-OWA-CANARY=_nP35uPsQkqVCZYQJGBugPD3xy9MfNgY1KM3Rz3wAJPU4RjIEzcUfkGAJNwZSEODB-LjjAeQaqI.&amp;token=eyJhbGciOiJSUzI1NiIsImtpZCI6IjU2MzU4ODUyMzRCOTI1MkRERTAwNTc2NkQ5RDlGMjc2NTY1RjYzRTIiLCJ0eXAiOiJKV1QiLCJ4NXQiOiJWaldJVWpTNUpTM2VBRmRtMmRueWRsWmZZLUkifQ.eyJvcmlnaW4iOiJodHRwczovL291dGxvb2sub2ZmaWNlLmNvbSIsInVjIjoiZWVmMTQ3NDllMzJjNGMxNWFlNjI0NzAzM2E0Yjg4ZTgiLCJzaWduaW5fc3RhdGUiOiJbXCJrbXNpXCJdIiwidmVyIjoiRXhjaGFuZ2UuQ2FsbGJhY2suVjEiLCJhcHBjdHhzZW5kZXIiOiJPd2FEb3dubG9hZEBjZDMxOTY3MS01MmU3LTRhNjgtYWZhOS1mY2Y4Zjg5ZjA5ZWEiLCJpc3NyaW5nIjoiV1ciLCJhcHBjdHgiOiJ7XCJtc2V4Y2hwcm90XCI6XCJvd2FcIixcInByaW1hcnlzaWRcIjpcIlMtMS01LTIxLTM5NzE5NTY3OC0xOTY5Njg2MjMxLTIyMjY0NjU5MC04MzkyOTc1XCIsXCJwdWlkXCI6XCIxMTUzODM2Mjk2MzE3ODYwMTg1XCIsXCJvaWRcIjpcIjFjYjEwZjM3LTc1MjgtNDQ2OS04YzU2LTcyM2YzNTEwNGVlYlwiLFwic2NvcGVcIjpcIk93YURvd25sb2FkXCJ9IiwibmJmIjoxNjA0MDA0MzAyLCJleHAiOjE2MDQwMDQ5MDIsImlzcyI6IjAwMDAwMDAyLTAwMDAtMGZmMS1jZTAwLTAwMDAwMDAwMDAwMEBjZDMxOTY3MS01MmU3LTRhNjgtYWZhOS1mY2Y4Zjg5ZjA5ZWEiLCJhdWQiOiIwMDAwMDAwMi0wMDAwLTBmZjEtY2UwMC0wMDAwMDAwMDAwMDAvYXR0YWNobWVudHMub2ZmaWNlLm5ldEBjZDMxOTY3MS01MmU3LTRhNjgtYWZhOS1mY2Y4Zjg5ZjA5ZWEiLCJoYXBwIjoib3dhIn0.gZ9dxAmPm3zZ0MELyOjVDXXmxIV7idcNLv-8Nycxs68J7cEtpokrH6P6CC74G_qaJlcxd2M7fxupSnalOGils37JnsMaaWoTh1Zrnulna2aCyiTgMuq16WZllTHGUajm_gQSygm4xslvqoI_YoJw8-2jqcOeTYaosC7wXXoCwUmsJv-emhWwn4APhcpmVvhPlQUExsktBZa_5-GiAPgNoE1zNqZfce8VSN1GTY-INW6wBUbXMPH1aDdgkKWoH6GnNagvEyteS0HCZNiOedm6ZGNpFjPg0Rf4l5Vnu8PIgcSC9oeKTGxXBeqWJQU-SdZeOhqEdtr755QqWBlcuZ9qdw&amp;animation=true">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000005000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -521,7 +553,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="6" name="Image 5" descr="https://attachments.office.net/owa/diana.mitchell%40mail.mcgill.ca/service.svc/s/GetAttachmentThumbnail?id=AAMkADc5MmE1MmYyLTdhNTUtNDhiNC05MzYzLWE1YjA5NWQyYzI0MwBGAAAAAADugN8DkS4MTL3ZuC%2B%2F5KU6BwB%2B5KHRNU0TSrhtGx73W2sFAAAABALUAAD7yC0FYtZ%2FRo4NqLo9fdP9AAK8QyQLAAABEgAQAFQvMGr%2BzwxEm3qxJy4NVDw%3D&amp;thumbnailType=2&amp;owa=outlook.office.com&amp;scriptVer=20201019001.14&amp;X-OWA-CANARY=_nP35uPsQkqVCZYQJGBugPD3xy9MfNgY1KM3Rz3wAJPU4RjIEzcUfkGAJNwZSEODB-LjjAeQaqI.&amp;token=eyJhbGciOiJSUzI1NiIsImtpZCI6IjU2MzU4ODUyMzRCOTI1MkRERTAwNTc2NkQ5RDlGMjc2NTY1RjYzRTIiLCJ0eXAiOiJKV1QiLCJ4NXQiOiJWaldJVWpTNUpTM2VBRmRtMmRueWRsWmZZLUkifQ.eyJvcmlnaW4iOiJodHRwczovL291dGxvb2sub2ZmaWNlLmNvbSIsInVjIjoiZWVmMTQ3NDllMzJjNGMxNWFlNjI0NzAzM2E0Yjg4ZTgiLCJzaWduaW5fc3RhdGUiOiJbXCJrbXNpXCJdIiwidmVyIjoiRXhjaGFuZ2UuQ2FsbGJhY2suVjEiLCJhcHBjdHhzZW5kZXIiOiJPd2FEb3dubG9hZEBjZDMxOTY3MS01MmU3LTRhNjgtYWZhOS1mY2Y4Zjg5ZjA5ZWEiLCJpc3NyaW5nIjoiV1ciLCJhcHBjdHgiOiJ7XCJtc2V4Y2hwcm90XCI6XCJvd2FcIixcInByaW1hcnlzaWRcIjpcIlMtMS01LTIxLTM5NzE5NTY3OC0xOTY5Njg2MjMxLTIyMjY0NjU5MC04MzkyOTc1XCIsXCJwdWlkXCI6XCIxMTUzODM2Mjk2MzE3ODYwMTg1XCIsXCJvaWRcIjpcIjFjYjEwZjM3LTc1MjgtNDQ2OS04YzU2LTcyM2YzNTEwNGVlYlwiLFwic2NvcGVcIjpcIk93YURvd25sb2FkXCJ9IiwibmJmIjoxNjA0MDA0MzAyLCJleHAiOjE2MDQwMDQ5MDIsImlzcyI6IjAwMDAwMDAyLTAwMDAtMGZmMS1jZTAwLTAwMDAwMDAwMDAwMEBjZDMxOTY3MS01MmU3LTRhNjgtYWZhOS1mY2Y4Zjg5ZjA5ZWEiLCJhdWQiOiIwMDAwMDAwMi0wMDAwLTBmZjEtY2UwMC0wMDAwMDAwMDAwMDAvYXR0YWNobWVudHMub2ZmaWNlLm5ldEBjZDMxOTY3MS01MmU3LTRhNjgtYWZhOS1mY2Y4Zjg5ZjA5ZWEiLCJoYXBwIjoib3dhIn0.gZ9dxAmPm3zZ0MELyOjVDXXmxIV7idcNLv-8Nycxs68J7cEtpokrH6P6CC74G_qaJlcxd2M7fxupSnalOGils37JnsMaaWoTh1Zrnulna2aCyiTgMuq16WZllTHGUajm_gQSygm4xslvqoI_YoJw8-2jqcOeTYaosC7wXXoCwUmsJv-emhWwn4APhcpmVvhPlQUExsktBZa_5-GiAPgNoE1zNqZfce8VSN1GTY-INW6wBUbXMPH1aDdgkKWoH6GnNagvEyteS0HCZNiOedm6ZGNpFjPg0Rf4l5Vnu8PIgcSC9oeKTGxXBeqWJQU-SdZeOhqEdtr755QqWBlcuZ9qdw&amp;animation=true"/>
+        <xdr:cNvPr id="6" name="Image 5" descr="https://attachments.office.net/owa/diana.mitchell%40mail.mcgill.ca/service.svc/s/GetAttachmentThumbnail?id=AAMkADc5MmE1MmYyLTdhNTUtNDhiNC05MzYzLWE1YjA5NWQyYzI0MwBGAAAAAADugN8DkS4MTL3ZuC%2B%2F5KU6BwB%2B5KHRNU0TSrhtGx73W2sFAAAABALUAAD7yC0FYtZ%2FRo4NqLo9fdP9AAK8QyQLAAABEgAQAFQvMGr%2BzwxEm3qxJy4NVDw%3D&amp;thumbnailType=2&amp;owa=outlook.office.com&amp;scriptVer=20201019001.14&amp;X-OWA-CANARY=_nP35uPsQkqVCZYQJGBugPD3xy9MfNgY1KM3Rz3wAJPU4RjIEzcUfkGAJNwZSEODB-LjjAeQaqI.&amp;token=eyJhbGciOiJSUzI1NiIsImtpZCI6IjU2MzU4ODUyMzRCOTI1MkRERTAwNTc2NkQ5RDlGMjc2NTY1RjYzRTIiLCJ0eXAiOiJKV1QiLCJ4NXQiOiJWaldJVWpTNUpTM2VBRmRtMmRueWRsWmZZLUkifQ.eyJvcmlnaW4iOiJodHRwczovL291dGxvb2sub2ZmaWNlLmNvbSIsInVjIjoiZWVmMTQ3NDllMzJjNGMxNWFlNjI0NzAzM2E0Yjg4ZTgiLCJzaWduaW5fc3RhdGUiOiJbXCJrbXNpXCJdIiwidmVyIjoiRXhjaGFuZ2UuQ2FsbGJhY2suVjEiLCJhcHBjdHhzZW5kZXIiOiJPd2FEb3dubG9hZEBjZDMxOTY3MS01MmU3LTRhNjgtYWZhOS1mY2Y4Zjg5ZjA5ZWEiLCJpc3NyaW5nIjoiV1ciLCJhcHBjdHgiOiJ7XCJtc2V4Y2hwcm90XCI6XCJvd2FcIixcInByaW1hcnlzaWRcIjpcIlMtMS01LTIxLTM5NzE5NTY3OC0xOTY5Njg2MjMxLTIyMjY0NjU5MC04MzkyOTc1XCIsXCJwdWlkXCI6XCIxMTUzODM2Mjk2MzE3ODYwMTg1XCIsXCJvaWRcIjpcIjFjYjEwZjM3LTc1MjgtNDQ2OS04YzU2LTcyM2YzNTEwNGVlYlwiLFwic2NvcGVcIjpcIk93YURvd25sb2FkXCJ9IiwibmJmIjoxNjA0MDA0MzAyLCJleHAiOjE2MDQwMDQ5MDIsImlzcyI6IjAwMDAwMDAyLTAwMDAtMGZmMS1jZTAwLTAwMDAwMDAwMDAwMEBjZDMxOTY3MS01MmU3LTRhNjgtYWZhOS1mY2Y4Zjg5ZjA5ZWEiLCJhdWQiOiIwMDAwMDAwMi0wMDAwLTBmZjEtY2UwMC0wMDAwMDAwMDAwMDAvYXR0YWNobWVudHMub2ZmaWNlLm5ldEBjZDMxOTY3MS01MmU3LTRhNjgtYWZhOS1mY2Y4Zjg5ZjA5ZWEiLCJoYXBwIjoib3dhIn0.gZ9dxAmPm3zZ0MELyOjVDXXmxIV7idcNLv-8Nycxs68J7cEtpokrH6P6CC74G_qaJlcxd2M7fxupSnalOGils37JnsMaaWoTh1Zrnulna2aCyiTgMuq16WZllTHGUajm_gQSygm4xslvqoI_YoJw8-2jqcOeTYaosC7wXXoCwUmsJv-emhWwn4APhcpmVvhPlQUExsktBZa_5-GiAPgNoE1zNqZfce8VSN1GTY-INW6wBUbXMPH1aDdgkKWoH6GnNagvEyteS0HCZNiOedm6ZGNpFjPg0Rf4l5Vnu8PIgcSC9oeKTGxXBeqWJQU-SdZeOhqEdtr755QqWBlcuZ9qdw&amp;animation=true">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000006000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -576,7 +614,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="7" name="Image 6" descr="https://attachments.office.net/owa/diana.mitchell%40mail.mcgill.ca/service.svc/s/GetAttachmentThumbnail?id=AAMkADc5MmE1MmYyLTdhNTUtNDhiNC05MzYzLWE1YjA5NWQyYzI0MwBGAAAAAADugN8DkS4MTL3ZuC%2B%2F5KU6BwB%2B5KHRNU0TSrhtGx73W2sFAAAABALUAAD7yC0FYtZ%2FRo4NqLo9fdP9AAK8QyQLAAABEgAQAMnDrJcsOJpBlh706a4eOUk%3D&amp;thumbnailType=2&amp;owa=outlook.office.com&amp;scriptVer=20201019001.14&amp;X-OWA-CANARY=_nP35uPsQkqVCZYQJGBugPD3xy9MfNgY1KM3Rz3wAJPU4RjIEzcUfkGAJNwZSEODB-LjjAeQaqI.&amp;token=eyJhbGciOiJSUzI1NiIsImtpZCI6IjU2MzU4ODUyMzRCOTI1MkRERTAwNTc2NkQ5RDlGMjc2NTY1RjYzRTIiLCJ0eXAiOiJKV1QiLCJ4NXQiOiJWaldJVWpTNUpTM2VBRmRtMmRueWRsWmZZLUkifQ.eyJvcmlnaW4iOiJodHRwczovL291dGxvb2sub2ZmaWNlLmNvbSIsInVjIjoiZWVmMTQ3NDllMzJjNGMxNWFlNjI0NzAzM2E0Yjg4ZTgiLCJzaWduaW5fc3RhdGUiOiJbXCJrbXNpXCJdIiwidmVyIjoiRXhjaGFuZ2UuQ2FsbGJhY2suVjEiLCJhcHBjdHhzZW5kZXIiOiJPd2FEb3dubG9hZEBjZDMxOTY3MS01MmU3LTRhNjgtYWZhOS1mY2Y4Zjg5ZjA5ZWEiLCJpc3NyaW5nIjoiV1ciLCJhcHBjdHgiOiJ7XCJtc2V4Y2hwcm90XCI6XCJvd2FcIixcInByaW1hcnlzaWRcIjpcIlMtMS01LTIxLTM5NzE5NTY3OC0xOTY5Njg2MjMxLTIyMjY0NjU5MC04MzkyOTc1XCIsXCJwdWlkXCI6XCIxMTUzODM2Mjk2MzE3ODYwMTg1XCIsXCJvaWRcIjpcIjFjYjEwZjM3LTc1MjgtNDQ2OS04YzU2LTcyM2YzNTEwNGVlYlwiLFwic2NvcGVcIjpcIk93YURvd25sb2FkXCJ9IiwibmJmIjoxNjA0MDA0MzAyLCJleHAiOjE2MDQwMDQ5MDIsImlzcyI6IjAwMDAwMDAyLTAwMDAtMGZmMS1jZTAwLTAwMDAwMDAwMDAwMEBjZDMxOTY3MS01MmU3LTRhNjgtYWZhOS1mY2Y4Zjg5ZjA5ZWEiLCJhdWQiOiIwMDAwMDAwMi0wMDAwLTBmZjEtY2UwMC0wMDAwMDAwMDAwMDAvYXR0YWNobWVudHMub2ZmaWNlLm5ldEBjZDMxOTY3MS01MmU3LTRhNjgtYWZhOS1mY2Y4Zjg5ZjA5ZWEiLCJoYXBwIjoib3dhIn0.gZ9dxAmPm3zZ0MELyOjVDXXmxIV7idcNLv-8Nycxs68J7cEtpokrH6P6CC74G_qaJlcxd2M7fxupSnalOGils37JnsMaaWoTh1Zrnulna2aCyiTgMuq16WZllTHGUajm_gQSygm4xslvqoI_YoJw8-2jqcOeTYaosC7wXXoCwUmsJv-emhWwn4APhcpmVvhPlQUExsktBZa_5-GiAPgNoE1zNqZfce8VSN1GTY-INW6wBUbXMPH1aDdgkKWoH6GnNagvEyteS0HCZNiOedm6ZGNpFjPg0Rf4l5Vnu8PIgcSC9oeKTGxXBeqWJQU-SdZeOhqEdtr755QqWBlcuZ9qdw&amp;animation=true"/>
+        <xdr:cNvPr id="7" name="Image 6" descr="https://attachments.office.net/owa/diana.mitchell%40mail.mcgill.ca/service.svc/s/GetAttachmentThumbnail?id=AAMkADc5MmE1MmYyLTdhNTUtNDhiNC05MzYzLWE1YjA5NWQyYzI0MwBGAAAAAADugN8DkS4MTL3ZuC%2B%2F5KU6BwB%2B5KHRNU0TSrhtGx73W2sFAAAABALUAAD7yC0FYtZ%2FRo4NqLo9fdP9AAK8QyQLAAABEgAQAMnDrJcsOJpBlh706a4eOUk%3D&amp;thumbnailType=2&amp;owa=outlook.office.com&amp;scriptVer=20201019001.14&amp;X-OWA-CANARY=_nP35uPsQkqVCZYQJGBugPD3xy9MfNgY1KM3Rz3wAJPU4RjIEzcUfkGAJNwZSEODB-LjjAeQaqI.&amp;token=eyJhbGciOiJSUzI1NiIsImtpZCI6IjU2MzU4ODUyMzRCOTI1MkRERTAwNTc2NkQ5RDlGMjc2NTY1RjYzRTIiLCJ0eXAiOiJKV1QiLCJ4NXQiOiJWaldJVWpTNUpTM2VBRmRtMmRueWRsWmZZLUkifQ.eyJvcmlnaW4iOiJodHRwczovL291dGxvb2sub2ZmaWNlLmNvbSIsInVjIjoiZWVmMTQ3NDllMzJjNGMxNWFlNjI0NzAzM2E0Yjg4ZTgiLCJzaWduaW5fc3RhdGUiOiJbXCJrbXNpXCJdIiwidmVyIjoiRXhjaGFuZ2UuQ2FsbGJhY2suVjEiLCJhcHBjdHhzZW5kZXIiOiJPd2FEb3dubG9hZEBjZDMxOTY3MS01MmU3LTRhNjgtYWZhOS1mY2Y4Zjg5ZjA5ZWEiLCJpc3NyaW5nIjoiV1ciLCJhcHBjdHgiOiJ7XCJtc2V4Y2hwcm90XCI6XCJvd2FcIixcInByaW1hcnlzaWRcIjpcIlMtMS01LTIxLTM5NzE5NTY3OC0xOTY5Njg2MjMxLTIyMjY0NjU5MC04MzkyOTc1XCIsXCJwdWlkXCI6XCIxMTUzODM2Mjk2MzE3ODYwMTg1XCIsXCJvaWRcIjpcIjFjYjEwZjM3LTc1MjgtNDQ2OS04YzU2LTcyM2YzNTEwNGVlYlwiLFwic2NvcGVcIjpcIk93YURvd25sb2FkXCJ9IiwibmJmIjoxNjA0MDA0MzAyLCJleHAiOjE2MDQwMDQ5MDIsImlzcyI6IjAwMDAwMDAyLTAwMDAtMGZmMS1jZTAwLTAwMDAwMDAwMDAwMEBjZDMxOTY3MS01MmU3LTRhNjgtYWZhOS1mY2Y4Zjg5ZjA5ZWEiLCJhdWQiOiIwMDAwMDAwMi0wMDAwLTBmZjEtY2UwMC0wMDAwMDAwMDAwMDAvYXR0YWNobWVudHMub2ZmaWNlLm5ldEBjZDMxOTY3MS01MmU3LTRhNjgtYWZhOS1mY2Y4Zjg5ZjA5ZWEiLCJoYXBwIjoib3dhIn0.gZ9dxAmPm3zZ0MELyOjVDXXmxIV7idcNLv-8Nycxs68J7cEtpokrH6P6CC74G_qaJlcxd2M7fxupSnalOGils37JnsMaaWoTh1Zrnulna2aCyiTgMuq16WZllTHGUajm_gQSygm4xslvqoI_YoJw8-2jqcOeTYaosC7wXXoCwUmsJv-emhWwn4APhcpmVvhPlQUExsktBZa_5-GiAPgNoE1zNqZfce8VSN1GTY-INW6wBUbXMPH1aDdgkKWoH6GnNagvEyteS0HCZNiOedm6ZGNpFjPg0Rf4l5Vnu8PIgcSC9oeKTGxXBeqWJQU-SdZeOhqEdtr755QqWBlcuZ9qdw&amp;animation=true">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000007000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -631,7 +675,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="8" name="Image 7" descr="https://attachments.office.net/owa/diana.mitchell%40mail.mcgill.ca/service.svc/s/GetAttachmentThumbnail?id=AAMkADc5MmE1MmYyLTdhNTUtNDhiNC05MzYzLWE1YjA5NWQyYzI0MwBGAAAAAADugN8DkS4MTL3ZuC%2B%2F5KU6BwB%2B5KHRNU0TSrhtGx73W2sFAAAABALUAAD7yC0FYtZ%2FRo4NqLo9fdP9AAK8QyQLAAABEgAQAMyU4iYYTD9NiJwAXfX369A%3D&amp;thumbnailType=2&amp;owa=outlook.office.com&amp;scriptVer=20201019001.14&amp;X-OWA-CANARY=_nP35uPsQkqVCZYQJGBugPD3xy9MfNgY1KM3Rz3wAJPU4RjIEzcUfkGAJNwZSEODB-LjjAeQaqI.&amp;token=eyJhbGciOiJSUzI1NiIsImtpZCI6IjU2MzU4ODUyMzRCOTI1MkRERTAwNTc2NkQ5RDlGMjc2NTY1RjYzRTIiLCJ0eXAiOiJKV1QiLCJ4NXQiOiJWaldJVWpTNUpTM2VBRmRtMmRueWRsWmZZLUkifQ.eyJvcmlnaW4iOiJodHRwczovL291dGxvb2sub2ZmaWNlLmNvbSIsInVjIjoiZWVmMTQ3NDllMzJjNGMxNWFlNjI0NzAzM2E0Yjg4ZTgiLCJzaWduaW5fc3RhdGUiOiJbXCJrbXNpXCJdIiwidmVyIjoiRXhjaGFuZ2UuQ2FsbGJhY2suVjEiLCJhcHBjdHhzZW5kZXIiOiJPd2FEb3dubG9hZEBjZDMxOTY3MS01MmU3LTRhNjgtYWZhOS1mY2Y4Zjg5ZjA5ZWEiLCJpc3NyaW5nIjoiV1ciLCJhcHBjdHgiOiJ7XCJtc2V4Y2hwcm90XCI6XCJvd2FcIixcInByaW1hcnlzaWRcIjpcIlMtMS01LTIxLTM5NzE5NTY3OC0xOTY5Njg2MjMxLTIyMjY0NjU5MC04MzkyOTc1XCIsXCJwdWlkXCI6XCIxMTUzODM2Mjk2MzE3ODYwMTg1XCIsXCJvaWRcIjpcIjFjYjEwZjM3LTc1MjgtNDQ2OS04YzU2LTcyM2YzNTEwNGVlYlwiLFwic2NvcGVcIjpcIk93YURvd25sb2FkXCJ9IiwibmJmIjoxNjA0MDA0MzAyLCJleHAiOjE2MDQwMDQ5MDIsImlzcyI6IjAwMDAwMDAyLTAwMDAtMGZmMS1jZTAwLTAwMDAwMDAwMDAwMEBjZDMxOTY3MS01MmU3LTRhNjgtYWZhOS1mY2Y4Zjg5ZjA5ZWEiLCJhdWQiOiIwMDAwMDAwMi0wMDAwLTBmZjEtY2UwMC0wMDAwMDAwMDAwMDAvYXR0YWNobWVudHMub2ZmaWNlLm5ldEBjZDMxOTY3MS01MmU3LTRhNjgtYWZhOS1mY2Y4Zjg5ZjA5ZWEiLCJoYXBwIjoib3dhIn0.gZ9dxAmPm3zZ0MELyOjVDXXmxIV7idcNLv-8Nycxs68J7cEtpokrH6P6CC74G_qaJlcxd2M7fxupSnalOGils37JnsMaaWoTh1Zrnulna2aCyiTgMuq16WZllTHGUajm_gQSygm4xslvqoI_YoJw8-2jqcOeTYaosC7wXXoCwUmsJv-emhWwn4APhcpmVvhPlQUExsktBZa_5-GiAPgNoE1zNqZfce8VSN1GTY-INW6wBUbXMPH1aDdgkKWoH6GnNagvEyteS0HCZNiOedm6ZGNpFjPg0Rf4l5Vnu8PIgcSC9oeKTGxXBeqWJQU-SdZeOhqEdtr755QqWBlcuZ9qdw&amp;animation=true"/>
+        <xdr:cNvPr id="8" name="Image 7" descr="https://attachments.office.net/owa/diana.mitchell%40mail.mcgill.ca/service.svc/s/GetAttachmentThumbnail?id=AAMkADc5MmE1MmYyLTdhNTUtNDhiNC05MzYzLWE1YjA5NWQyYzI0MwBGAAAAAADugN8DkS4MTL3ZuC%2B%2F5KU6BwB%2B5KHRNU0TSrhtGx73W2sFAAAABALUAAD7yC0FYtZ%2FRo4NqLo9fdP9AAK8QyQLAAABEgAQAMyU4iYYTD9NiJwAXfX369A%3D&amp;thumbnailType=2&amp;owa=outlook.office.com&amp;scriptVer=20201019001.14&amp;X-OWA-CANARY=_nP35uPsQkqVCZYQJGBugPD3xy9MfNgY1KM3Rz3wAJPU4RjIEzcUfkGAJNwZSEODB-LjjAeQaqI.&amp;token=eyJhbGciOiJSUzI1NiIsImtpZCI6IjU2MzU4ODUyMzRCOTI1MkRERTAwNTc2NkQ5RDlGMjc2NTY1RjYzRTIiLCJ0eXAiOiJKV1QiLCJ4NXQiOiJWaldJVWpTNUpTM2VBRmRtMmRueWRsWmZZLUkifQ.eyJvcmlnaW4iOiJodHRwczovL291dGxvb2sub2ZmaWNlLmNvbSIsInVjIjoiZWVmMTQ3NDllMzJjNGMxNWFlNjI0NzAzM2E0Yjg4ZTgiLCJzaWduaW5fc3RhdGUiOiJbXCJrbXNpXCJdIiwidmVyIjoiRXhjaGFuZ2UuQ2FsbGJhY2suVjEiLCJhcHBjdHhzZW5kZXIiOiJPd2FEb3dubG9hZEBjZDMxOTY3MS01MmU3LTRhNjgtYWZhOS1mY2Y4Zjg5ZjA5ZWEiLCJpc3NyaW5nIjoiV1ciLCJhcHBjdHgiOiJ7XCJtc2V4Y2hwcm90XCI6XCJvd2FcIixcInByaW1hcnlzaWRcIjpcIlMtMS01LTIxLTM5NzE5NTY3OC0xOTY5Njg2MjMxLTIyMjY0NjU5MC04MzkyOTc1XCIsXCJwdWlkXCI6XCIxMTUzODM2Mjk2MzE3ODYwMTg1XCIsXCJvaWRcIjpcIjFjYjEwZjM3LTc1MjgtNDQ2OS04YzU2LTcyM2YzNTEwNGVlYlwiLFwic2NvcGVcIjpcIk93YURvd25sb2FkXCJ9IiwibmJmIjoxNjA0MDA0MzAyLCJleHAiOjE2MDQwMDQ5MDIsImlzcyI6IjAwMDAwMDAyLTAwMDAtMGZmMS1jZTAwLTAwMDAwMDAwMDAwMEBjZDMxOTY3MS01MmU3LTRhNjgtYWZhOS1mY2Y4Zjg5ZjA5ZWEiLCJhdWQiOiIwMDAwMDAwMi0wMDAwLTBmZjEtY2UwMC0wMDAwMDAwMDAwMDAvYXR0YWNobWVudHMub2ZmaWNlLm5ldEBjZDMxOTY3MS01MmU3LTRhNjgtYWZhOS1mY2Y4Zjg5ZjA5ZWEiLCJoYXBwIjoib3dhIn0.gZ9dxAmPm3zZ0MELyOjVDXXmxIV7idcNLv-8Nycxs68J7cEtpokrH6P6CC74G_qaJlcxd2M7fxupSnalOGils37JnsMaaWoTh1Zrnulna2aCyiTgMuq16WZllTHGUajm_gQSygm4xslvqoI_YoJw8-2jqcOeTYaosC7wXXoCwUmsJv-emhWwn4APhcpmVvhPlQUExsktBZa_5-GiAPgNoE1zNqZfce8VSN1GTY-INW6wBUbXMPH1aDdgkKWoH6GnNagvEyteS0HCZNiOedm6ZGNpFjPg0Rf4l5Vnu8PIgcSC9oeKTGxXBeqWJQU-SdZeOhqEdtr755QqWBlcuZ9qdw&amp;animation=true">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000008000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -686,7 +736,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="9" name="Image 8" descr="https://attachments.office.net/owa/diana.mitchell%40mail.mcgill.ca/service.svc/s/GetAttachmentThumbnail?id=AAMkADc5MmE1MmYyLTdhNTUtNDhiNC05MzYzLWE1YjA5NWQyYzI0MwBGAAAAAADugN8DkS4MTL3ZuC%2B%2F5KU6BwB%2B5KHRNU0TSrhtGx73W2sFAAAABALUAAD7yC0FYtZ%2FRo4NqLo9fdP9AAK8QyQLAAABEgAQAMUX0A8CgqpJh5rYQMg4PTE%3D&amp;thumbnailType=2&amp;owa=outlook.office.com&amp;scriptVer=20201019001.14&amp;X-OWA-CANARY=s-GIdMSD7EOUAWUnM2B8h5CAaltMfNgY2hvNNqRnNqhZ6cG1td9koUAgV4HcYk4_S-KNUU_i1jQ.&amp;token=eyJhbGciOiJSUzI1NiIsImtpZCI6IjU2MzU4ODUyMzRCOTI1MkRERTAwNTc2NkQ5RDlGMjc2NTY1RjYzRTIiLCJ0eXAiOiJKV1QiLCJ4NXQiOiJWaldJVWpTNUpTM2VBRmRtMmRueWRsWmZZLUkifQ.eyJvcmlnaW4iOiJodHRwczovL291dGxvb2sub2ZmaWNlLmNvbSIsInVjIjoiZWVmMTQ3NDllMzJjNGMxNWFlNjI0NzAzM2E0Yjg4ZTgiLCJzaWduaW5fc3RhdGUiOiJbXCJrbXNpXCJdIiwidmVyIjoiRXhjaGFuZ2UuQ2FsbGJhY2suVjEiLCJhcHBjdHhzZW5kZXIiOiJPd2FEb3dubG9hZEBjZDMxOTY3MS01MmU3LTRhNjgtYWZhOS1mY2Y4Zjg5ZjA5ZWEiLCJpc3NyaW5nIjoiV1ciLCJhcHBjdHgiOiJ7XCJtc2V4Y2hwcm90XCI6XCJvd2FcIixcInByaW1hcnlzaWRcIjpcIlMtMS01LTIxLTM5NzE5NTY3OC0xOTY5Njg2MjMxLTIyMjY0NjU5MC04MzkyOTc1XCIsXCJwdWlkXCI6XCIxMTUzODM2Mjk2MzE3ODYwMTg1XCIsXCJvaWRcIjpcIjFjYjEwZjM3LTc1MjgtNDQ2OS04YzU2LTcyM2YzNTEwNGVlYlwiLFwic2NvcGVcIjpcIk93YURvd25sb2FkXCJ9IiwibmJmIjoxNjA0MDA0NjA1LCJleHAiOjE2MDQwMDUyMDUsImlzcyI6IjAwMDAwMDAyLTAwMDAtMGZmMS1jZTAwLTAwMDAwMDAwMDAwMEBjZDMxOTY3MS01MmU3LTRhNjgtYWZhOS1mY2Y4Zjg5ZjA5ZWEiLCJhdWQiOiIwMDAwMDAwMi0wMDAwLTBmZjEtY2UwMC0wMDAwMDAwMDAwMDAvYXR0YWNobWVudHMub2ZmaWNlLm5ldEBjZDMxOTY3MS01MmU3LTRhNjgtYWZhOS1mY2Y4Zjg5ZjA5ZWEiLCJoYXBwIjoib3dhIn0.Rabx1khZxtnZzkubMmntrYIChAKkYpEkdRSdyDYgniVzbwV29DNWDZ9FEX2cVmOdrp8kZBFUlYzqh5-GqVozbNYa6r82Pp9-WQRB5JO0hg1D8s8EvbjRQuZrA0INCBD7EWcxyjPhdEWRavrHnxGAb4qFYGScLBrcXrQ3eteK46W-UfEGDjwGQjOfGh6_MQs-kyXKC_s9PcWPmcEKlRR9-UAffMbIbnb7cNCAdPc_V9aEcM56LF7bqkA8c9exY91uUn2dfJXmgnQbCEQIC8o3mgbw4wILM4riiS60BXZxypJm6bGMjm4e0fIK4dhw8MQpmfXzCv5b7L_DV7Bbmd8Hlg&amp;animation=true"/>
+        <xdr:cNvPr id="9" name="Image 8" descr="https://attachments.office.net/owa/diana.mitchell%40mail.mcgill.ca/service.svc/s/GetAttachmentThumbnail?id=AAMkADc5MmE1MmYyLTdhNTUtNDhiNC05MzYzLWE1YjA5NWQyYzI0MwBGAAAAAADugN8DkS4MTL3ZuC%2B%2F5KU6BwB%2B5KHRNU0TSrhtGx73W2sFAAAABALUAAD7yC0FYtZ%2FRo4NqLo9fdP9AAK8QyQLAAABEgAQAMUX0A8CgqpJh5rYQMg4PTE%3D&amp;thumbnailType=2&amp;owa=outlook.office.com&amp;scriptVer=20201019001.14&amp;X-OWA-CANARY=s-GIdMSD7EOUAWUnM2B8h5CAaltMfNgY2hvNNqRnNqhZ6cG1td9koUAgV4HcYk4_S-KNUU_i1jQ.&amp;token=eyJhbGciOiJSUzI1NiIsImtpZCI6IjU2MzU4ODUyMzRCOTI1MkRERTAwNTc2NkQ5RDlGMjc2NTY1RjYzRTIiLCJ0eXAiOiJKV1QiLCJ4NXQiOiJWaldJVWpTNUpTM2VBRmRtMmRueWRsWmZZLUkifQ.eyJvcmlnaW4iOiJodHRwczovL291dGxvb2sub2ZmaWNlLmNvbSIsInVjIjoiZWVmMTQ3NDllMzJjNGMxNWFlNjI0NzAzM2E0Yjg4ZTgiLCJzaWduaW5fc3RhdGUiOiJbXCJrbXNpXCJdIiwidmVyIjoiRXhjaGFuZ2UuQ2FsbGJhY2suVjEiLCJhcHBjdHhzZW5kZXIiOiJPd2FEb3dubG9hZEBjZDMxOTY3MS01MmU3LTRhNjgtYWZhOS1mY2Y4Zjg5ZjA5ZWEiLCJpc3NyaW5nIjoiV1ciLCJhcHBjdHgiOiJ7XCJtc2V4Y2hwcm90XCI6XCJvd2FcIixcInByaW1hcnlzaWRcIjpcIlMtMS01LTIxLTM5NzE5NTY3OC0xOTY5Njg2MjMxLTIyMjY0NjU5MC04MzkyOTc1XCIsXCJwdWlkXCI6XCIxMTUzODM2Mjk2MzE3ODYwMTg1XCIsXCJvaWRcIjpcIjFjYjEwZjM3LTc1MjgtNDQ2OS04YzU2LTcyM2YzNTEwNGVlYlwiLFwic2NvcGVcIjpcIk93YURvd25sb2FkXCJ9IiwibmJmIjoxNjA0MDA0NjA1LCJleHAiOjE2MDQwMDUyMDUsImlzcyI6IjAwMDAwMDAyLTAwMDAtMGZmMS1jZTAwLTAwMDAwMDAwMDAwMEBjZDMxOTY3MS01MmU3LTRhNjgtYWZhOS1mY2Y4Zjg5ZjA5ZWEiLCJhdWQiOiIwMDAwMDAwMi0wMDAwLTBmZjEtY2UwMC0wMDAwMDAwMDAwMDAvYXR0YWNobWVudHMub2ZmaWNlLm5ldEBjZDMxOTY3MS01MmU3LTRhNjgtYWZhOS1mY2Y4Zjg5ZjA5ZWEiLCJoYXBwIjoib3dhIn0.Rabx1khZxtnZzkubMmntrYIChAKkYpEkdRSdyDYgniVzbwV29DNWDZ9FEX2cVmOdrp8kZBFUlYzqh5-GqVozbNYa6r82Pp9-WQRB5JO0hg1D8s8EvbjRQuZrA0INCBD7EWcxyjPhdEWRavrHnxGAb4qFYGScLBrcXrQ3eteK46W-UfEGDjwGQjOfGh6_MQs-kyXKC_s9PcWPmcEKlRR9-UAffMbIbnb7cNCAdPc_V9aEcM56LF7bqkA8c9exY91uUn2dfJXmgnQbCEQIC8o3mgbw4wILM4riiS60BXZxypJm6bGMjm4e0fIK4dhw8MQpmfXzCv5b7L_DV7Bbmd8Hlg&amp;animation=true">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000009000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -991,29 +1047,29 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:P11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A2:P11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="9" max="9" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="L2" s="19" t="s">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="L2" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="M2" s="19"/>
-      <c r="N2" s="19"/>
-      <c r="O2" s="19"/>
-      <c r="P2" s="19"/>
+      <c r="M2" s="17"/>
+      <c r="N2" s="17"/>
+      <c r="O2" s="17"/>
+      <c r="P2" s="17"/>
     </row>
-    <row r="3" spans="2:16" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="B3" s="3" t="s">
         <v>17</v>
       </c>
@@ -1038,7 +1094,7 @@
       <c r="I3" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="K3" s="14" t="s">
+      <c r="K3" s="11" t="s">
         <v>24</v>
       </c>
       <c r="L3" s="3">
@@ -1057,7 +1113,10 @@
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>1</v>
+      </c>
       <c r="B4" s="1" t="s">
         <v>11</v>
       </c>
@@ -1082,7 +1141,8 @@
       <c r="I4" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="K4" s="15" t="s">
+      <c r="J4" s="18"/>
+      <c r="K4" s="12" t="s">
         <v>25</v>
       </c>
       <c r="L4" s="1">
@@ -1101,7 +1161,10 @@
         <v>160</v>
       </c>
     </row>
-    <row r="5" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>6</v>
+      </c>
       <c r="B5" s="1" t="s">
         <v>12</v>
       </c>
@@ -1126,7 +1189,7 @@
       <c r="I5" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="K5" s="16" t="s">
+      <c r="K5" s="13" t="s">
         <v>25</v>
       </c>
       <c r="L5" s="1">
@@ -1145,7 +1208,10 @@
         <v>168</v>
       </c>
     </row>
-    <row r="6" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>2</v>
+      </c>
       <c r="B6" s="1" t="s">
         <v>13</v>
       </c>
@@ -1170,16 +1236,19 @@
       <c r="I6" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="K6" s="17" t="s">
+      <c r="K6" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="L6" s="20"/>
-      <c r="M6" s="20"/>
-      <c r="N6" s="20"/>
-      <c r="O6" s="20"/>
-      <c r="P6" s="20"/>
+      <c r="L6" s="16"/>
+      <c r="M6" s="16"/>
+      <c r="N6" s="16"/>
+      <c r="O6" s="16"/>
+      <c r="P6" s="16"/>
     </row>
-    <row r="7" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>3</v>
+      </c>
       <c r="B7" s="1" t="s">
         <v>14</v>
       </c>
@@ -1204,7 +1273,7 @@
       <c r="I7" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="K7" s="18" t="s">
+      <c r="K7" s="15" t="s">
         <v>26</v>
       </c>
       <c r="L7" s="1"/>
@@ -1213,7 +1282,10 @@
       <c r="O7" s="1"/>
       <c r="P7" s="1"/>
     </row>
-    <row r="8" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>4</v>
+      </c>
       <c r="B8" s="1" t="s">
         <v>15</v>
       </c>
@@ -1238,7 +1310,7 @@
       <c r="I8" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="K8" s="18" t="s">
+      <c r="K8" s="15" t="s">
         <v>26</v>
       </c>
       <c r="L8" s="1"/>
@@ -1247,7 +1319,10 @@
       <c r="O8" s="1"/>
       <c r="P8" s="1"/>
     </row>
-    <row r="9" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>5</v>
+      </c>
       <c r="B9" s="1" t="s">
         <v>16</v>
       </c>
@@ -1272,7 +1347,7 @@
       <c r="I9" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="K9" s="18" t="s">
+      <c r="K9" s="15" t="s">
         <v>26</v>
       </c>
       <c r="L9" s="1"/>
@@ -1281,32 +1356,32 @@
       <c r="O9" s="1"/>
       <c r="P9" s="1"/>
     </row>
-    <row r="11" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B11" s="10" t="s">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B11" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="10" t="s">
+      <c r="C11" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D11" s="11">
+      <c r="D11" s="5">
         <v>25.34</v>
       </c>
-      <c r="E11" s="11">
+      <c r="E11" s="5">
         <v>39.450000000000003</v>
       </c>
-      <c r="F11" s="11">
+      <c r="F11" s="5">
         <v>17.88</v>
       </c>
-      <c r="G11" s="11">
+      <c r="G11" s="5">
         <v>0.45</v>
       </c>
       <c r="H11" s="6">
         <v>0.16</v>
       </c>
-      <c r="I11" s="12" t="s">
+      <c r="I11" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="K11" s="13" t="s">
+      <c r="K11" s="10" t="s">
         <v>25</v>
       </c>
       <c r="L11" s="1">
@@ -1335,14 +1410,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+    <sheetView topLeftCell="I40" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
       <selection activeCell="F113" sqref="F113"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>